<commit_message>
feat: Add Commercial column for user assignment in full imports
Allow assigning customers to specific users via email in the Commercial column:

- Add "Commercial" column (M) to import_complet_exemple.xlsx
- Parse commercial_email from Excel (supports "Commercial" or "Email Commercial" headers)
- Assign customer to user by email if provided, null if empty (new customers only)
- Keep existing assignment for existing customers when column is empty
- Track commercial changes in import analysis (case-insensitive email comparison)
- Add tests for commercial assignment verification

Behavior:
- Column filled with email: Assign customer to that user
- Column filled with invalid email: Log warning, set to null
- Column empty (new customer): Leave unassigned (null)
- Column empty (existing customer): Keep existing assignment
</commit_message>
<xml_diff>
--- a/public/examples/import_complet_exemple.xlsx
+++ b/public/examples/import_complet_exemple.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>Raison Sociale</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>Recherche économies d'énergie</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>admin@test.com</t>
+  </si>
+  <si>
+    <t>user@test.com</t>
   </si>
   <si>
     <t>INSTRUCTIONS POUR L'IMPORT COMPLET</t>
@@ -588,7 +597,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:L1"/>
@@ -596,21 +605,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="8.712" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="36.42" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="16.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="29.421" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="35.277" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="26.993" customWidth="true" style="0"/>
+    <col min="2" max="2" width="17.567" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8.712" customWidth="true" style="0"/>
+    <col min="4" max="4" width="9.283" customWidth="true" style="0"/>
+    <col min="5" max="5" width="36.42" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12.854" customWidth="true" style="0"/>
+    <col min="7" max="7" width="17.567" customWidth="true" style="0"/>
+    <col min="8" max="8" width="17.567" customWidth="true" style="0"/>
+    <col min="9" max="9" width="16.567" customWidth="true" style="0"/>
+    <col min="10" max="10" width="12.854" customWidth="true" style="0"/>
+    <col min="11" max="11" width="29.421" customWidth="true" style="0"/>
+    <col min="12" max="12" width="35.277" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,8 +656,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -685,8 +697,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -723,8 +738,11 @@
       <c r="L3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -787,147 +805,142 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1"/>
+        <v>44</v>
+      </c>
+    </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1"/>
+        <v>46</v>
+      </c>
+    </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1"/>
+        <v>58</v>
+      </c>
+    </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1"/>
+        <v>61</v>
+      </c>
+    </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1"/>
+        <v>65</v>
+      </c>
+    </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
style: Fix code style with PHP-CS-Fixer
</commit_message>
<xml_diff>
--- a/public/examples/import_complet_exemple.xlsx
+++ b/public/examples/import_complet_exemple.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
   <si>
     <t>Raison Sociale</t>
   </si>
@@ -139,15 +139,6 @@
   </si>
   <si>
     <t>Recherche économies d'énergie</t>
-  </si>
-  <si>
-    <t>Commercial</t>
-  </si>
-  <si>
-    <t>admin@test.com</t>
-  </si>
-  <si>
-    <t>user@test.com</t>
   </si>
   <si>
     <t>INSTRUCTIONS POUR L'IMPORT COMPLET</t>
@@ -597,7 +588,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:L1"/>
@@ -605,21 +596,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.993" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567" customWidth="true" style="0"/>
-    <col min="3" max="3" width="8.712" customWidth="true" style="0"/>
-    <col min="4" max="4" width="9.283" customWidth="true" style="0"/>
-    <col min="5" max="5" width="36.42" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12.854" customWidth="true" style="0"/>
-    <col min="7" max="7" width="17.567" customWidth="true" style="0"/>
-    <col min="8" max="8" width="17.567" customWidth="true" style="0"/>
-    <col min="9" max="9" width="16.567" customWidth="true" style="0"/>
-    <col min="10" max="10" width="12.854" customWidth="true" style="0"/>
-    <col min="11" max="11" width="29.421" customWidth="true" style="0"/>
-    <col min="12" max="12" width="35.277" customWidth="true" style="0"/>
+    <col min="1" max="1" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8.712" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="36.42" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="16.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="29.421" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="35.277" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,11 +647,8 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -697,11 +685,8 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -738,11 +723,8 @@
       <c r="L3" t="s">
         <v>31</v>
       </c>
-      <c r="M3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -805,142 +787,147 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1"/>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>46</v>
-      </c>
-    </row>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1"/>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>58</v>
-      </c>
-    </row>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1"/>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>61</v>
-      </c>
-    </row>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1"/>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>65</v>
-      </c>
-    </row>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1"/>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Add Commercial column to import example file
</commit_message>
<xml_diff>
--- a/public/examples/import_complet_exemple.xlsx
+++ b/public/examples/import_complet_exemple.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>Raison Sociale</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>Recherche économies d'énergie</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>admin@test.com</t>
+  </si>
+  <si>
+    <t>user@test.com</t>
   </si>
   <si>
     <t>INSTRUCTIONS POUR L'IMPORT COMPLET</t>
@@ -588,7 +597,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:L1"/>
@@ -596,21 +605,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="8.712" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="36.42" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="16.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="29.421" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="35.277" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="26.993" customWidth="true" style="0"/>
+    <col min="2" max="2" width="17.567" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8.712" customWidth="true" style="0"/>
+    <col min="4" max="4" width="9.283" customWidth="true" style="0"/>
+    <col min="5" max="5" width="36.42" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12.854" customWidth="true" style="0"/>
+    <col min="7" max="7" width="17.567" customWidth="true" style="0"/>
+    <col min="8" max="8" width="17.567" customWidth="true" style="0"/>
+    <col min="9" max="9" width="16.567" customWidth="true" style="0"/>
+    <col min="10" max="10" width="12.854" customWidth="true" style="0"/>
+    <col min="11" max="11" width="29.421" customWidth="true" style="0"/>
+    <col min="12" max="12" width="35.277" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,8 +656,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -685,8 +697,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -723,8 +738,11 @@
       <c r="L3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -787,147 +805,142 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1"/>
+        <v>44</v>
+      </c>
+    </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1"/>
+        <v>46</v>
+      </c>
+    </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1"/>
+        <v>58</v>
+      </c>
+    </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1"/>
+        <v>61</v>
+      </c>
+    </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1"/>
+        <v>65</v>
+      </c>
+    </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: Mise à jour des fichiers d'exemple d'import Excel
- Mise à jour des 4 fichiers d'exemple d'import
- Ajout de la colonne Commercial dans les exemples
- Synchronisation avec les nouveaux headers supportés
</commit_message>
<xml_diff>
--- a/public/examples/import_complet_exemple.xlsx
+++ b/public/examples/import_complet_exemple.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
   <si>
     <t>Raison Sociale</t>
   </si>
@@ -139,15 +139,6 @@
   </si>
   <si>
     <t>Recherche économies d'énergie</t>
-  </si>
-  <si>
-    <t>Commercial</t>
-  </si>
-  <si>
-    <t>admin@test.com</t>
-  </si>
-  <si>
-    <t>user@test.com</t>
   </si>
   <si>
     <t>INSTRUCTIONS POUR L'IMPORT COMPLET</t>
@@ -597,7 +588,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:L1"/>
@@ -605,21 +596,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.993" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567" customWidth="true" style="0"/>
-    <col min="3" max="3" width="8.712" customWidth="true" style="0"/>
-    <col min="4" max="4" width="9.283" customWidth="true" style="0"/>
-    <col min="5" max="5" width="36.42" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12.854" customWidth="true" style="0"/>
-    <col min="7" max="7" width="17.567" customWidth="true" style="0"/>
-    <col min="8" max="8" width="17.567" customWidth="true" style="0"/>
-    <col min="9" max="9" width="16.567" customWidth="true" style="0"/>
-    <col min="10" max="10" width="12.854" customWidth="true" style="0"/>
-    <col min="11" max="11" width="29.421" customWidth="true" style="0"/>
-    <col min="12" max="12" width="35.277" customWidth="true" style="0"/>
+    <col min="1" max="1" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8.712" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="36.42" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="16.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="29.421" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="35.277" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,11 +647,8 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -697,11 +685,8 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -738,11 +723,8 @@
       <c r="L3" t="s">
         <v>31</v>
       </c>
-      <c r="M3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -805,142 +787,147 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1"/>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>46</v>
-      </c>
-    </row>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1"/>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>58</v>
-      </c>
-    </row>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1"/>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>61</v>
-      </c>
-    </row>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1"/>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>65</v>
-      </c>
-    </row>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1"/>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>